<commit_message>
mods to context files and creation of a new one, fix to isajson.py relates to issue #414, fix to isatab.py for compatibility with pandas1.3.4 relates to issue #428, adding a test to json2jsonld.py for ttl conversion
</commit_message>
<xml_diff>
--- a/isatools/resources/json-context/mapping_file.xlsx
+++ b/isatools/resources/json-context/mapping_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippe/Documents/git/isa-api2/isa-api/isatools/resources/json-context/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EE0B13-D29B-EA44-A408-B8CA5D8DE17E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7D436F-4B32-0B47-A897-ECA597035914}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{3D64FA27-1BDC-CD43-A7D7-9761B2358A50}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
   <si>
     <t>Comment</t>
   </si>
@@ -253,6 +253,72 @@
   </si>
   <si>
     <t>isa</t>
+  </si>
+  <si>
+    <t>isaterms</t>
+  </si>
+  <si>
+    <t>assay_type</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>factor_value</t>
+  </si>
+  <si>
+    <t>investigation</t>
+  </si>
+  <si>
+    <t>characteristic</t>
+  </si>
+  <si>
+    <t>characteristic_value</t>
+  </si>
+  <si>
+    <t>ontology_annotation</t>
+  </si>
+  <si>
+    <t>ontology</t>
+  </si>
+  <si>
+    <t>organization</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>parameter_value</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>protocol_parameter</t>
+  </si>
+  <si>
+    <t>publication</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>material_entity</t>
   </si>
 </sst>
 </file>
@@ -604,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FDA0A5-4B40-7C4B-AF06-93DD3DFBAD1F}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +683,7 @@
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -630,8 +696,11 @@
       <c r="D1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -644,8 +713,11 @@
       <c r="D2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -658,8 +730,11 @@
       <c r="D3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -672,8 +747,11 @@
       <c r="D4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -686,8 +764,11 @@
       <c r="D5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -700,8 +781,11 @@
       <c r="D6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -714,8 +798,11 @@
       <c r="D7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -728,8 +815,11 @@
       <c r="D8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -742,8 +832,11 @@
       <c r="D9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -756,8 +849,11 @@
       <c r="D10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -770,8 +866,11 @@
       <c r="D11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -784,8 +883,11 @@
       <c r="D12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -798,8 +900,11 @@
       <c r="D13" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -812,8 +917,11 @@
       <c r="D14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -826,8 +934,11 @@
       <c r="D15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -840,8 +951,11 @@
       <c r="D16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -854,8 +968,11 @@
       <c r="D17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -868,8 +985,11 @@
       <c r="D18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -882,8 +1002,11 @@
       <c r="D19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -896,8 +1019,11 @@
       <c r="D20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -910,8 +1036,11 @@
       <c r="D21" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -924,8 +1053,11 @@
       <c r="D22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -937,6 +1069,9 @@
       </c>
       <c r="D23" t="s">
         <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>